<commit_message>
Update code and excel sheet for TC71808
# Conflicts:
#	Test Scripts/NGConsys/Libraries/PSULoad_Functions.cs
</commit_message>
<xml_diff>
--- a/Test Data/TC_71808_Verify_Normal_Load_On_Changing_Housing_Property_Of_DIM_FC.xlsx
+++ b/Test Data/TC_71808_Verify_Normal_Load_On_Changing_Housing_Property_Of_DIM_FC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310806E5-2B3A-4A6A-9F4B-5E8C7F0E4738}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459FB613-54F4-4D87-AD65-A2FE59717D17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,10 +151,10 @@
     <t>Ancillary Conventional</t>
   </si>
   <si>
+    <t>Battery load</t>
+  </si>
+  <si>
     <t>Class B - 1 Spur</t>
-  </si>
-  <si>
-    <t>Battery load</t>
   </si>
 </sst>
 </file>
@@ -318,6 +318,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -329,18 +341,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,12 +647,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -662,10 +662,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -707,7 +707,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
         <v>26</v>
@@ -722,20 +722,20 @@
         <v>0.05</v>
       </c>
       <c r="J6" s="17"/>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="24"/>
+      <c r="L6" s="28"/>
       <c r="N6" s="17">
         <v>0.251</v>
       </c>
       <c r="O6" s="17">
         <v>0.443</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="24"/>
+      <c r="R6" s="28"/>
     </row>
     <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -780,7 +780,7 @@
       <c r="N7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="28" t="s">
+      <c r="O7" s="24" t="s">
         <v>32</v>
       </c>
       <c r="Q7" s="19" t="s">
@@ -797,7 +797,7 @@
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -806,10 +806,10 @@
       <c r="E8" s="6">
         <v>16</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="22">
         <v>0.25</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="23">
         <v>0.438</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -828,7 +828,7 @@
         <v>0.443</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N8" s="20">
         <v>0.25</v>

</xml_diff>